<commit_message>
now writing a zero to GDX
</commit_message>
<xml_diff>
--- a/sandbox/sv.xlsx
+++ b/sandbox/sv.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="75" windowWidth="26835" windowHeight="11310" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="75" windowWidth="26835" windowHeight="11310"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="24">
   <si>
     <t>dset</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>process with "gdxxrw sv.xlsx output=xvxls.gdx index=index!a1 Squeeze=N"</t>
+  </si>
+  <si>
+    <t>squeeze=N</t>
   </si>
 </sst>
 </file>
@@ -424,15 +427,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="18.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
         <v>9</v>
       </c>
@@ -440,34 +446,39 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="D3">
+      <c r="D4">
         <v>2</v>
       </c>
-      <c r="E3">
+      <c r="E4">
         <v>2</v>
       </c>
     </row>
@@ -480,7 +491,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>

</xml_diff>